<commit_message>
First/Second Examiner Pages Updated
</commit_message>
<xml_diff>
--- a/ERP-BlazorApp/ERP.BlazorUI/wwwroot/exports/IS1420_TakeHome12_Results.xlsx
+++ b/ERP-BlazorApp/ERP.BlazorUI/wwwroot/exports/IS1420_TakeHome12_Results.xlsx
@@ -493,9 +493,9 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="18.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="13.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="13.085625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="18.085625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="13.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3">

</xml_diff>